<commit_message>
Function Updates in Lime Explanation Code
</commit_message>
<xml_diff>
--- a/Learning Rates.xlsx
+++ b/Learning Rates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\65860\Desktop\SoftwareEngineering\Year2\ITP\Project\Traffic_ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E9C5C7-A263-4E69-AB6A-F78F388D2703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B145E1BE-4729-46BB-8EBD-70ECE1E63A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F5510DF6-6AEA-43BD-A05A-616AF09602DE}"/>
   </bookViews>
@@ -147,12 +147,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
     <numFmt numFmtId="166" formatCode="0.00000%"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +183,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -248,7 +256,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -332,19 +340,18 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -357,15 +364,555 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="74">
+  <dxfs count="139">
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.00000%"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.0000%"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -391,292 +938,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="166" formatCode="0.00000%"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="0.0000%"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2407,8 +2668,8 @@
     <dataField name="Accuracy Average" fld="11" subtotal="average" baseField="3" baseItem="1" numFmtId="10"/>
     <dataField name="Loss Average" fld="10" subtotal="average" baseField="4" baseItem="0" numFmtId="10"/>
   </dataFields>
-  <formats count="29">
-    <format dxfId="73">
+  <formats count="77">
+    <format dxfId="138">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1">
@@ -2417,7 +2678,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="137">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1">
@@ -2426,7 +2687,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="136">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -2435,7 +2696,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="135">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4" count="2">
@@ -2448,7 +2709,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
+    <format dxfId="134">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4" count="1">
@@ -2460,7 +2721,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="133">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -2469,7 +2730,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="67">
+    <format dxfId="132">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -2478,7 +2739,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="66">
+    <format dxfId="131">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -2487,7 +2748,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="65">
+    <format dxfId="130">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -2496,7 +2757,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="64">
+    <format dxfId="129">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4" count="1">
@@ -2508,7 +2769,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="63">
+    <format dxfId="128">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4" count="1">
@@ -2520,7 +2781,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="62">
+    <format dxfId="127">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4" count="1">
@@ -2532,7 +2793,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="61">
+    <format dxfId="126">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="1">
@@ -2541,7 +2802,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="60">
+    <format dxfId="125">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -2550,7 +2811,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="59">
+    <format dxfId="124">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="2" selected="0">
@@ -2563,7 +2824,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="123">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2572,7 +2833,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="57">
+    <format dxfId="122">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="2">
@@ -2585,7 +2846,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="56">
+    <format dxfId="121">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="2" selected="0">
@@ -2598,7 +2859,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="55">
+    <format dxfId="120">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -2606,6 +2867,190 @@
           </reference>
         </references>
       </pivotArea>
+    </format>
+    <format dxfId="119">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="118">
+      <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="117">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="116">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="0" selected="0"/>
+          <reference field="5" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="115">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="0" selected="0"/>
+          <reference field="5" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="114">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="0" selected="0"/>
+          <reference field="5" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="113">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="0" selected="0"/>
+          <reference field="5" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="112">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="0" selected="0"/>
+          <reference field="5" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="111">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="110">
+      <pivotArea field="3" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="64">
+      <pivotArea field="3" dataOnly="0" labelOnly="1" grandCol="1" outline="0" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="62">
+      <pivotArea field="3" dataOnly="0" labelOnly="1" grandCol="1" outline="0" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="60">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="59">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="58">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="57">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
     <format dxfId="54">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
@@ -2615,16 +3060,20 @@
             <x v="1"/>
           </reference>
           <reference field="3" count="1" selected="0">
-            <x v="1"/>
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="53">
-      <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="2"/>
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -2642,91 +3091,601 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="51">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+    <format dxfId="49">
+      <pivotArea field="3" dataOnly="0" labelOnly="1" grandCol="1" outline="0" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="47">
+      <pivotArea field="3" dataOnly="0" labelOnly="1" grandCol="1" outline="0" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="45">
+      <pivotArea field="5" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="1">
         <references count="3">
           <reference field="4294967294" count="2" selected="0">
             <x v="0"/>
             <x v="1"/>
           </reference>
-          <reference field="3" count="0" selected="0"/>
+          <reference field="4" count="1" selected="0">
+            <x v="4"/>
+          </reference>
           <reference field="5" count="1">
             <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="50">
+    <format dxfId="44">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="42">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
-          <reference field="4294967294" count="2" selected="0">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
             <x v="0"/>
-            <x v="1"/>
-          </reference>
-          <reference field="3" count="0" selected="0"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="40">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
           <reference field="5" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="49">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="38">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
-          <reference field="4294967294" count="2" selected="0">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
             <x v="0"/>
-            <x v="1"/>
-          </reference>
-          <reference field="3" count="0" selected="0"/>
-          <reference field="5" count="1">
+          </reference>
+          <reference field="4" count="1">
             <x v="2"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="36">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="5" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="34">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
-          <reference field="4294967294" count="2" selected="0">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
             <x v="0"/>
-            <x v="1"/>
-          </reference>
-          <reference field="3" count="0" selected="0"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="32">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="3"/>
+          </reference>
           <reference field="5" count="1">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="47">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="30">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
-          <reference field="4294967294" count="2" selected="0">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
             <x v="0"/>
-            <x v="1"/>
-          </reference>
-          <reference field="3" count="0" selected="0"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="28">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="4"/>
+          </reference>
           <reference field="5" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="26">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="25">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="24">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="23">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="22">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="5" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="21">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="20">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="19">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1">
             <x v="4"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
-      <pivotArea outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
+    <format dxfId="18">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="5" count="1">
             <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
-      <pivotArea field="3" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="2" selected="0">
+    <format dxfId="17">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
             <x v="0"/>
-            <x v="1"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="16">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="15">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="14">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="13">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="5" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="12">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="11">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea field="5" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="1">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea field="4" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea field="5" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="1">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea field="4" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea field="5" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="1">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="5" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea field="4" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea field="5" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="1">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea field="4" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea field="5" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="1">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -2819,23 +3778,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{716538A6-ED17-40C4-B673-F6A22A5DF3AB}" name="Table4" displayName="Table4" ref="B4:J14" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{716538A6-ED17-40C4-B673-F6A22A5DF3AB}" name="Table4" displayName="Table4" ref="B4:J14" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108">
   <autoFilter ref="B4:J14" xr:uid="{716538A6-ED17-40C4-B673-F6A22A5DF3AB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:J14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{6EA67E11-5EF1-4F64-8BF9-939BD93D1040}" name="Feature Extraction" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{22CDFD67-B970-45A7-87A1-66E85E671FF3}" name="Fine Tuning" dataDxfId="41" dataCellStyle="Percent">
+    <tableColumn id="1" xr3:uid="{6EA67E11-5EF1-4F64-8BF9-939BD93D1040}" name="Feature Extraction" dataDxfId="107"/>
+    <tableColumn id="2" xr3:uid="{22CDFD67-B970-45A7-87A1-66E85E671FF3}" name="Fine Tuning" dataDxfId="106" dataCellStyle="Percent">
       <calculatedColumnFormula>B5/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C25C17D1-21B9-4655-B69D-96CD06F9BA58}" name="Epoch Set" dataDxfId="40" dataCellStyle="Percent"/>
-    <tableColumn id="5" xr3:uid="{466B42DB-1E9E-4715-8191-AC1258ABD07E}" name="Epoch Undergo" dataDxfId="39" dataCellStyle="Percent"/>
-    <tableColumn id="6" xr3:uid="{78B26499-9791-444B-82E2-CC6BB1F58B87}" name="Epoch SetFT" dataDxfId="38" dataCellStyle="Percent"/>
-    <tableColumn id="7" xr3:uid="{6065AA55-BC9E-4401-BE42-91F91100B40D}" name="Epoch UndergoFT" dataDxfId="37" dataCellStyle="Percent"/>
-    <tableColumn id="9" xr3:uid="{0D9DEFB1-5291-4E76-8E60-33993FC8A74A}" name="Test Dataset Loss" dataDxfId="36" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{A5FE943B-77B2-48AD-80B3-6ACCA0283617}" name="Test Dataset Accuracy" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{8585E09E-BE35-48A6-989E-910542286FC9}" name="Correct Predictions (Out of 59)" dataDxfId="34" dataCellStyle="Percent">
+    <tableColumn id="4" xr3:uid="{C25C17D1-21B9-4655-B69D-96CD06F9BA58}" name="Epoch Set" dataDxfId="105" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{466B42DB-1E9E-4715-8191-AC1258ABD07E}" name="Epoch Undergo" dataDxfId="104" dataCellStyle="Percent"/>
+    <tableColumn id="6" xr3:uid="{78B26499-9791-444B-82E2-CC6BB1F58B87}" name="Epoch SetFT" dataDxfId="103" dataCellStyle="Percent"/>
+    <tableColumn id="7" xr3:uid="{6065AA55-BC9E-4401-BE42-91F91100B40D}" name="Epoch UndergoFT" dataDxfId="102" dataCellStyle="Percent"/>
+    <tableColumn id="9" xr3:uid="{0D9DEFB1-5291-4E76-8E60-33993FC8A74A}" name="Test Dataset Loss" dataDxfId="101" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{A5FE943B-77B2-48AD-80B3-6ACCA0283617}" name="Test Dataset Accuracy" dataDxfId="100"/>
+    <tableColumn id="8" xr3:uid="{8585E09E-BE35-48A6-989E-910542286FC9}" name="Correct Predictions (Out of 59)" dataDxfId="99" dataCellStyle="Percent">
       <calculatedColumnFormula>59*Table4[[#This Row],[Test Dataset Accuracy]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2844,33 +3803,33 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7F2F301C-5A38-4540-B768-F8EE0DF5A255}" name="Table42" displayName="Table42" ref="B17:P27" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7F2F301C-5A38-4540-B768-F8EE0DF5A255}" name="Table42" displayName="Table42" ref="B17:P27" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97">
   <autoFilter ref="B17:P27" xr:uid="{7F2F301C-5A38-4540-B768-F8EE0DF5A255}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B18:P27">
     <sortCondition ref="B17:B27"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{485E10B5-49B3-4B34-B2A8-8DB25F38CDCA}" name="Feature Extraction" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{4F0EFF3C-EFBD-4D81-AF1E-B70D89FE1140}" name="Fine Tuning" dataDxfId="30" dataCellStyle="Percent">
+    <tableColumn id="1" xr3:uid="{485E10B5-49B3-4B34-B2A8-8DB25F38CDCA}" name="Feature Extraction" dataDxfId="96"/>
+    <tableColumn id="2" xr3:uid="{4F0EFF3C-EFBD-4D81-AF1E-B70D89FE1140}" name="Fine Tuning" dataDxfId="95" dataCellStyle="Percent">
       <calculatedColumnFormula>B18/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77EF4E9A-34E8-42B4-8650-6D0269E36D3D}" name="Epoch Set" dataDxfId="29" dataCellStyle="Percent"/>
-    <tableColumn id="5" xr3:uid="{3737EB52-8EE7-42AC-BCF5-DACF8AB4C666}" name="Epoch Undergo" dataDxfId="28" dataCellStyle="Percent"/>
-    <tableColumn id="6" xr3:uid="{DCEDF8C3-7222-4373-9998-716476D1DC64}" name="Epoch SetFT" dataDxfId="27" dataCellStyle="Percent"/>
-    <tableColumn id="7" xr3:uid="{74AAFDFC-BD4D-486D-AAA8-27D289481B92}" name="Epoch UndergoFT" dataDxfId="26" dataCellStyle="Percent"/>
-    <tableColumn id="9" xr3:uid="{43302B6C-0A80-40E6-B114-66E468306993}" name="Loss1" dataDxfId="25" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{26356F77-460D-416A-99B3-BBF85C9DC69C}" name="Accuracy1" dataDxfId="24"/>
-    <tableColumn id="10" xr3:uid="{33DD8E20-21E9-42DB-A9ED-2EB6254B6694}" name="Loss2" dataDxfId="23"/>
-    <tableColumn id="11" xr3:uid="{6829DF2F-21F4-45FB-AA73-F683252A3142}" name="Accuracy2" dataDxfId="22"/>
-    <tableColumn id="12" xr3:uid="{5F661F4D-678B-4020-A679-2664CA8B6202}" name="Loss3" dataDxfId="21"/>
-    <tableColumn id="13" xr3:uid="{C3FA50CB-D03F-46D8-8412-C9DB34573DBE}" name="Accuracy3" dataDxfId="20"/>
-    <tableColumn id="14" xr3:uid="{8A397EB8-90C6-4673-BA0C-2881AB360A11}" name="Average Loss" dataDxfId="19">
+    <tableColumn id="4" xr3:uid="{77EF4E9A-34E8-42B4-8650-6D0269E36D3D}" name="Epoch Set" dataDxfId="94" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{3737EB52-8EE7-42AC-BCF5-DACF8AB4C666}" name="Epoch Undergo" dataDxfId="93" dataCellStyle="Percent"/>
+    <tableColumn id="6" xr3:uid="{DCEDF8C3-7222-4373-9998-716476D1DC64}" name="Epoch SetFT" dataDxfId="92" dataCellStyle="Percent"/>
+    <tableColumn id="7" xr3:uid="{74AAFDFC-BD4D-486D-AAA8-27D289481B92}" name="Epoch UndergoFT" dataDxfId="91" dataCellStyle="Percent"/>
+    <tableColumn id="9" xr3:uid="{43302B6C-0A80-40E6-B114-66E468306993}" name="Loss1" dataDxfId="90" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{26356F77-460D-416A-99B3-BBF85C9DC69C}" name="Accuracy1" dataDxfId="89"/>
+    <tableColumn id="10" xr3:uid="{33DD8E20-21E9-42DB-A9ED-2EB6254B6694}" name="Loss2" dataDxfId="88"/>
+    <tableColumn id="11" xr3:uid="{6829DF2F-21F4-45FB-AA73-F683252A3142}" name="Accuracy2" dataDxfId="87"/>
+    <tableColumn id="12" xr3:uid="{5F661F4D-678B-4020-A679-2664CA8B6202}" name="Loss3" dataDxfId="86"/>
+    <tableColumn id="13" xr3:uid="{C3FA50CB-D03F-46D8-8412-C9DB34573DBE}" name="Accuracy3" dataDxfId="85"/>
+    <tableColumn id="14" xr3:uid="{8A397EB8-90C6-4673-BA0C-2881AB360A11}" name="Average Loss" dataDxfId="84">
       <calculatedColumnFormula>SUM(Table42[[#This Row],[Loss1]],Table42[[#This Row],[Loss2]],Table42[[#This Row],[Loss3]])/3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{38831F4B-7CB6-47D1-8189-BC480F70AD1C}" name="Average Accuracy" dataDxfId="18">
+    <tableColumn id="15" xr3:uid="{38831F4B-7CB6-47D1-8189-BC480F70AD1C}" name="Average Accuracy" dataDxfId="83">
       <calculatedColumnFormula>SUM(Table42[[#This Row],[Accuracy1]],Table42[[#This Row],[Accuracy2]],Table42[[#This Row],[Accuracy3]])/3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2104EC55-481A-4232-AE55-D62BBCD49840}" name="Correct Predictions (Out of 59)" dataDxfId="17" dataCellStyle="Percent">
+    <tableColumn id="8" xr3:uid="{2104EC55-481A-4232-AE55-D62BBCD49840}" name="Correct Predictions (Out of 59)" dataDxfId="82" dataCellStyle="Percent">
       <calculatedColumnFormula>59*Table42[[#This Row],[Accuracy1]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2879,22 +3838,22 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{81E28367-2AA6-4DC8-ABBD-1124D9E224C3}" name="Table2" displayName="Table2" ref="B31:N58" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{81E28367-2AA6-4DC8-ABBD-1124D9E224C3}" name="Table2" displayName="Table2" ref="B31:N58" totalsRowShown="0" headerRowDxfId="81" dataDxfId="79" headerRowBorderDxfId="80" tableBorderDxfId="78">
   <autoFilter ref="B31:N58" xr:uid="{81E28367-2AA6-4DC8-ABBD-1124D9E224C3}"/>
   <tableColumns count="13">
-    <tableColumn id="18" xr3:uid="{15CAC9F2-A9AE-4DF9-9463-27879ABEF874}" name="S/N" dataDxfId="2"/>
-    <tableColumn id="20" xr3:uid="{8751364B-A1F1-4231-839D-41D6BB3744A9}" name="Learning Rate Category" dataDxfId="0"/>
-    <tableColumn id="17" xr3:uid="{88D66E1E-4B55-479B-8E01-B940A81D996D}" name="Group" dataDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{C29B4EA7-872E-4985-985F-D1263991876A}" name="Attempt" dataDxfId="12"/>
-    <tableColumn id="1" xr3:uid="{74E818B4-0889-4479-B54B-2EB291E76806}" name="Feature Extraction" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{E88A4247-AE56-4CAC-ADE1-2DC704DFF04C}" name="Fine Tuning" dataDxfId="10" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{2D1A8174-0CF5-49BA-A3D3-35867E5CEF7A}" name="Epoch Set" dataDxfId="9" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{B2813A48-925E-4FF2-9D9E-34A17D47193E}" name="Epoch Undergo" dataDxfId="8" dataCellStyle="Percent"/>
-    <tableColumn id="5" xr3:uid="{2B60C0D8-8FA3-49FB-BBB4-167EEE24539A}" name="Epoch SetFT" dataDxfId="7" dataCellStyle="Percent"/>
-    <tableColumn id="6" xr3:uid="{E9B28B45-1179-4DAB-BC0E-B365B8833F0E}" name="Epoch UndergoFT" dataDxfId="6" dataCellStyle="Percent"/>
-    <tableColumn id="7" xr3:uid="{2754ABEE-B570-4C31-9C72-7C21A1F82BA4}" name="Loss" dataDxfId="5" dataCellStyle="Percent"/>
-    <tableColumn id="8" xr3:uid="{2913B544-8DB0-45C7-9420-367138A8248F}" name="Accuracy" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{F30FA38B-490A-4BE9-8DB2-AD16F3E68C1C}" name="Correct Predictions (Out of 59)" dataDxfId="3" dataCellStyle="Percent">
+    <tableColumn id="18" xr3:uid="{15CAC9F2-A9AE-4DF9-9463-27879ABEF874}" name="S/N" dataDxfId="77"/>
+    <tableColumn id="20" xr3:uid="{8751364B-A1F1-4231-839D-41D6BB3744A9}" name="Learning Rate Category" dataDxfId="76"/>
+    <tableColumn id="17" xr3:uid="{88D66E1E-4B55-479B-8E01-B940A81D996D}" name="Group" dataDxfId="75"/>
+    <tableColumn id="19" xr3:uid="{C29B4EA7-872E-4985-985F-D1263991876A}" name="Attempt" dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{74E818B4-0889-4479-B54B-2EB291E76806}" name="Feature Extraction" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{E88A4247-AE56-4CAC-ADE1-2DC704DFF04C}" name="Fine Tuning" dataDxfId="72" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{2D1A8174-0CF5-49BA-A3D3-35867E5CEF7A}" name="Epoch Set" dataDxfId="71" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{B2813A48-925E-4FF2-9D9E-34A17D47193E}" name="Epoch Undergo" dataDxfId="70" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{2B60C0D8-8FA3-49FB-BBB4-167EEE24539A}" name="Epoch SetFT" dataDxfId="69" dataCellStyle="Percent"/>
+    <tableColumn id="6" xr3:uid="{E9B28B45-1179-4DAB-BC0E-B365B8833F0E}" name="Epoch UndergoFT" dataDxfId="68" dataCellStyle="Percent"/>
+    <tableColumn id="7" xr3:uid="{2754ABEE-B570-4C31-9C72-7C21A1F82BA4}" name="Loss" dataDxfId="67" dataCellStyle="Percent"/>
+    <tableColumn id="8" xr3:uid="{2913B544-8DB0-45C7-9420-367138A8248F}" name="Accuracy" dataDxfId="66"/>
+    <tableColumn id="15" xr3:uid="{F30FA38B-490A-4BE9-8DB2-AD16F3E68C1C}" name="Correct Predictions (Out of 59)" dataDxfId="65" dataCellStyle="Percent">
       <calculatedColumnFormula>59*Table2[[#This Row],[Accuracy]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3202,21 +4161,16 @@
   <dimension ref="B2:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.77734375" customWidth="1"/>
     <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="10.77734375" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
     <col min="11" max="11" width="7.33203125" customWidth="1"/>
     <col min="12" max="12" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
@@ -3308,88 +4262,90 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C5" s="33">
+    <row r="5" spans="2:10" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="32">
         <v>1</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="36">
+      <c r="D5" s="32"/>
+      <c r="E5" s="33">
         <v>2</v>
       </c>
-      <c r="F5" s="36"/>
-      <c r="G5" s="39">
+      <c r="F5" s="33"/>
+      <c r="G5" s="34">
         <v>3</v>
       </c>
-      <c r="H5" s="39"/>
-      <c r="I5" t="s">
+      <c r="H5" s="34"/>
+      <c r="I5" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="51" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="39" t="s">
+      <c r="H6" s="43" t="s">
         <v>29</v>
       </c>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="29">
         <v>8.0000000000000007E-5</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="30">
         <v>7.9999999999999996E-6</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="48">
         <v>0.89829999999999999</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="53">
         <v>0.35570000000000002</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="49">
         <v>0.89829999999999999</v>
       </c>
-      <c r="F8" s="38">
+      <c r="F8" s="55">
         <v>0.2923</v>
       </c>
-      <c r="G8" s="41">
+      <c r="G8" s="50">
         <v>0.86439999999999995</v>
       </c>
-      <c r="H8" s="41">
+      <c r="H8" s="57">
         <v>0.32619999999999999</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="47">
         <v>0.88700000000000001</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="59">
         <v>0.32473333333333332</v>
       </c>
     </row>
@@ -3397,41 +4353,41 @@
       <c r="B9" s="29">
         <v>9.0000000000000006E-5</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="59"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="30">
         <v>7.9999999999999996E-6</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="48">
         <v>0.88139999999999996</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="53">
         <v>0.31280000000000002</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="49">
         <v>0.88139999999999996</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="55">
         <v>0.32579999999999998</v>
       </c>
-      <c r="G10" s="41">
+      <c r="G10" s="50">
         <v>0.9153</v>
       </c>
-      <c r="H10" s="41">
+      <c r="H10" s="57">
         <v>0.34310000000000002</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I10" s="47">
         <v>0.89269999999999994</v>
       </c>
-      <c r="J10" s="31">
+      <c r="J10" s="59">
         <v>0.32723333333333332</v>
       </c>
     </row>
@@ -3439,41 +4395,41 @@
       <c r="B11" s="29">
         <v>1E-4</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="59"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="30">
         <v>7.9999999999999996E-6</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="48">
         <v>0.88139999999999996</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D12" s="53">
         <v>0.34820000000000001</v>
       </c>
-      <c r="E12" s="38">
+      <c r="E12" s="49">
         <v>0.88139999999999996</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F12" s="55">
         <v>0.33729999999999999</v>
       </c>
-      <c r="G12" s="41">
+      <c r="G12" s="50">
         <v>0.88139999999999996</v>
       </c>
-      <c r="H12" s="41">
+      <c r="H12" s="57">
         <v>0.3115</v>
       </c>
-      <c r="I12" s="31">
+      <c r="I12" s="47">
         <v>0.88139999999999985</v>
       </c>
-      <c r="J12" s="31">
+      <c r="J12" s="59">
         <v>0.33233333333333331</v>
       </c>
     </row>
@@ -3481,28 +4437,28 @@
       <c r="B13" s="30">
         <v>9.0000000000000002E-6</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="48">
         <v>0.84750000000000003</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="53">
         <v>0.3276</v>
       </c>
-      <c r="E13" s="38">
+      <c r="E13" s="49">
         <v>0.89829999999999999</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="55">
         <v>0.34</v>
       </c>
-      <c r="G13" s="41">
+      <c r="G13" s="50">
         <v>0.88139999999999996</v>
       </c>
-      <c r="H13" s="41">
+      <c r="H13" s="57">
         <v>0.28820000000000001</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I13" s="47">
         <v>0.87573333333333336</v>
       </c>
-      <c r="J13" s="31">
+      <c r="J13" s="59">
         <v>0.31859999999999999</v>
       </c>
     </row>
@@ -3510,28 +4466,28 @@
       <c r="B14" s="30">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="48">
         <v>0.83099999999999996</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="53">
         <v>0.318</v>
       </c>
-      <c r="E14" s="38">
+      <c r="E14" s="49">
         <v>0.86439999999999995</v>
       </c>
-      <c r="F14" s="38">
+      <c r="F14" s="55">
         <v>0.36280000000000001</v>
       </c>
-      <c r="G14" s="41">
+      <c r="G14" s="50">
         <v>0.86439999999999995</v>
       </c>
-      <c r="H14" s="41">
+      <c r="H14" s="57">
         <v>0.29389999999999999</v>
       </c>
-      <c r="I14" s="31">
+      <c r="I14" s="47">
         <v>0.85326666666666651</v>
       </c>
-      <c r="J14" s="31">
+      <c r="J14" s="59">
         <v>0.32490000000000002</v>
       </c>
     </row>
@@ -3539,28 +4495,28 @@
       <c r="B15" s="30">
         <v>1.1E-5</v>
       </c>
-      <c r="C15" s="35">
+      <c r="C15" s="48">
         <v>0.81359999999999999</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D15" s="53">
         <v>0.28499999999999998</v>
       </c>
-      <c r="E15" s="38">
+      <c r="E15" s="49">
         <v>0.86439999999999995</v>
       </c>
-      <c r="F15" s="38">
+      <c r="F15" s="55">
         <v>0.28220000000000001</v>
       </c>
-      <c r="G15" s="41">
+      <c r="G15" s="50">
         <v>0.89829999999999999</v>
       </c>
-      <c r="H15" s="41">
+      <c r="H15" s="57">
         <v>0.2928</v>
       </c>
-      <c r="I15" s="31">
+      <c r="I15" s="47">
         <v>0.85876666666666657</v>
       </c>
-      <c r="J15" s="31">
+      <c r="J15" s="59">
         <v>0.28666666666666663</v>
       </c>
     </row>
@@ -3568,28 +4524,28 @@
       <c r="B16" s="30">
         <v>1.2E-5</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="48">
         <v>0.88139999999999996</v>
       </c>
-      <c r="D16" s="35">
+      <c r="D16" s="53">
         <v>0.27060000000000001</v>
       </c>
-      <c r="E16" s="38">
+      <c r="E16" s="49">
         <v>0.86439999999999995</v>
       </c>
-      <c r="F16" s="38">
+      <c r="F16" s="55">
         <v>0.33379999999999999</v>
       </c>
-      <c r="G16" s="41">
+      <c r="G16" s="50">
         <v>0.88139999999999996</v>
       </c>
-      <c r="H16" s="41">
+      <c r="H16" s="57">
         <v>0.31330000000000002</v>
       </c>
-      <c r="I16" s="31">
+      <c r="I16" s="47">
         <v>0.87573333333333336</v>
       </c>
-      <c r="J16" s="31">
+      <c r="J16" s="59">
         <v>0.30590000000000001</v>
       </c>
     </row>
@@ -3597,41 +4553,41 @@
       <c r="B17" s="29">
         <v>1.1E-4</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="59"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="30">
         <v>7.9999999999999996E-6</v>
       </c>
-      <c r="C18" s="35">
+      <c r="C18" s="48">
         <v>0.81359999999999999</v>
       </c>
-      <c r="D18" s="35">
+      <c r="D18" s="53">
         <v>0.3266</v>
       </c>
-      <c r="E18" s="38">
+      <c r="E18" s="49">
         <v>0.83050000000000002</v>
       </c>
-      <c r="F18" s="38">
+      <c r="F18" s="55">
         <v>0.36230000000000001</v>
       </c>
-      <c r="G18" s="41">
+      <c r="G18" s="50">
         <v>0.83050000000000002</v>
       </c>
-      <c r="H18" s="41">
+      <c r="H18" s="57">
         <v>0.33050000000000002</v>
       </c>
-      <c r="I18" s="31">
+      <c r="I18" s="47">
         <v>0.82486666666666653</v>
       </c>
-      <c r="J18" s="31">
+      <c r="J18" s="59">
         <v>0.33980000000000005</v>
       </c>
     </row>
@@ -3639,46 +4595,47 @@
       <c r="B19" s="29">
         <v>1.2E-4</v>
       </c>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="59"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="30">
         <v>7.9999999999999996E-6</v>
       </c>
-      <c r="C20" s="35">
+      <c r="C20" s="48">
         <v>0.89829999999999999</v>
       </c>
-      <c r="D20" s="35">
+      <c r="D20" s="53">
         <v>0.31469999999999998</v>
       </c>
-      <c r="E20" s="38">
+      <c r="E20" s="49">
         <v>0.9153</v>
       </c>
-      <c r="F20" s="38">
+      <c r="F20" s="55">
         <v>0.26700000000000002</v>
       </c>
-      <c r="G20" s="41">
+      <c r="G20" s="50">
         <v>0.88139999999999996</v>
       </c>
-      <c r="H20" s="41">
+      <c r="H20" s="57">
         <v>0.28820000000000001</v>
       </c>
-      <c r="I20" s="31">
+      <c r="I20" s="52">
         <v>0.89833333333333343</v>
       </c>
-      <c r="J20" s="31">
+      <c r="J20" s="60">
         <v>0.28996666666666665</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3708,31 +4665,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="2:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="43" t="s">
+      <c r="C3" s="37"/>
+      <c r="D3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44" t="s">
+      <c r="E3" s="38"/>
+      <c r="F3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="44"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="2:10" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -4078,18 +5035,18 @@
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="2:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="43" t="s">
+      <c r="C16" s="37"/>
+      <c r="D16" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="43"/>
-      <c r="F16" s="44" t="s">
+      <c r="E16" s="38"/>
+      <c r="F16" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="44"/>
+      <c r="G16" s="39"/>
     </row>
     <row r="17" spans="2:16" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B17" s="12" t="s">
@@ -4593,16 +5550,16 @@
       </c>
     </row>
     <row r="32" spans="2:16" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="32">
+      <c r="B32" s="31">
         <v>1</v>
       </c>
-      <c r="C32" s="46" t="s">
+      <c r="C32" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="32">
+      <c r="D32" s="31">
         <v>1</v>
       </c>
-      <c r="E32" s="32">
+      <c r="E32" s="31">
         <v>1</v>
       </c>
       <c r="F32" s="18">
@@ -4635,16 +5592,16 @@
       </c>
     </row>
     <row r="33" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="32">
+      <c r="B33" s="31">
         <v>2</v>
       </c>
-      <c r="C33" s="46" t="s">
+      <c r="C33" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="32">
+      <c r="D33" s="31">
         <v>1</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E33" s="31">
         <v>2</v>
       </c>
       <c r="F33" s="18">
@@ -4677,16 +5634,16 @@
       </c>
     </row>
     <row r="34" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="32">
+      <c r="B34" s="31">
         <v>3</v>
       </c>
-      <c r="C34" s="46" t="s">
+      <c r="C34" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="32">
+      <c r="D34" s="31">
         <v>1</v>
       </c>
-      <c r="E34" s="32">
+      <c r="E34" s="31">
         <v>3</v>
       </c>
       <c r="F34" s="18">
@@ -4719,16 +5676,16 @@
       </c>
     </row>
     <row r="35" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="32">
+      <c r="B35" s="31">
         <v>4</v>
       </c>
-      <c r="C35" s="46" t="s">
+      <c r="C35" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="32">
+      <c r="D35" s="31">
         <v>2</v>
       </c>
-      <c r="E35" s="32">
+      <c r="E35" s="31">
         <v>1</v>
       </c>
       <c r="F35" s="18">
@@ -4761,16 +5718,16 @@
       </c>
     </row>
     <row r="36" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="32">
+      <c r="B36" s="31">
         <v>5</v>
       </c>
-      <c r="C36" s="46" t="s">
+      <c r="C36" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="32">
+      <c r="D36" s="31">
         <v>2</v>
       </c>
-      <c r="E36" s="32">
+      <c r="E36" s="31">
         <v>2</v>
       </c>
       <c r="F36" s="18">
@@ -4803,16 +5760,16 @@
       </c>
     </row>
     <row r="37" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="32">
+      <c r="B37" s="31">
         <v>6</v>
       </c>
-      <c r="C37" s="46" t="s">
+      <c r="C37" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="32">
+      <c r="D37" s="31">
         <v>2</v>
       </c>
-      <c r="E37" s="32">
+      <c r="E37" s="31">
         <v>3</v>
       </c>
       <c r="F37" s="18">
@@ -4845,16 +5802,16 @@
       </c>
     </row>
     <row r="38" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="32">
+      <c r="B38" s="31">
         <v>7</v>
       </c>
-      <c r="C38" s="46" t="s">
+      <c r="C38" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D38" s="32">
+      <c r="D38" s="31">
         <v>3</v>
       </c>
-      <c r="E38" s="32">
+      <c r="E38" s="31">
         <v>1</v>
       </c>
       <c r="F38" s="18">
@@ -4887,16 +5844,16 @@
       </c>
     </row>
     <row r="39" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="32">
+      <c r="B39" s="31">
         <v>8</v>
       </c>
-      <c r="C39" s="46" t="s">
+      <c r="C39" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="32">
+      <c r="D39" s="31">
         <v>3</v>
       </c>
-      <c r="E39" s="32">
+      <c r="E39" s="31">
         <v>2</v>
       </c>
       <c r="F39" s="18">
@@ -4929,16 +5886,16 @@
       </c>
     </row>
     <row r="40" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="32">
+      <c r="B40" s="31">
         <v>9</v>
       </c>
-      <c r="C40" s="46" t="s">
+      <c r="C40" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D40" s="32">
+      <c r="D40" s="31">
         <v>3</v>
       </c>
-      <c r="E40" s="32">
+      <c r="E40" s="31">
         <v>3</v>
       </c>
       <c r="F40" s="18">
@@ -4971,16 +5928,16 @@
       </c>
     </row>
     <row r="41" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="32">
+      <c r="B41" s="31">
         <v>10</v>
       </c>
-      <c r="C41" s="46" t="s">
+      <c r="C41" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="32">
+      <c r="D41" s="31">
         <v>4</v>
       </c>
-      <c r="E41" s="32">
+      <c r="E41" s="31">
         <v>1</v>
       </c>
       <c r="F41" s="18">
@@ -5013,16 +5970,16 @@
       </c>
     </row>
     <row r="42" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="32">
+      <c r="B42" s="31">
         <v>11</v>
       </c>
-      <c r="C42" s="46" t="s">
+      <c r="C42" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D42" s="32">
+      <c r="D42" s="31">
         <v>4</v>
       </c>
-      <c r="E42" s="32">
+      <c r="E42" s="31">
         <v>2</v>
       </c>
       <c r="F42" s="18">
@@ -5055,16 +6012,16 @@
       </c>
     </row>
     <row r="43" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="32">
+      <c r="B43" s="31">
         <v>12</v>
       </c>
-      <c r="C43" s="46" t="s">
+      <c r="C43" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D43" s="32">
+      <c r="D43" s="31">
         <v>4</v>
       </c>
-      <c r="E43" s="32">
+      <c r="E43" s="31">
         <v>3</v>
       </c>
       <c r="F43" s="18">
@@ -5097,16 +6054,16 @@
       </c>
     </row>
     <row r="44" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="32">
+      <c r="B44" s="31">
         <v>13</v>
       </c>
-      <c r="C44" s="46" t="s">
+      <c r="C44" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D44" s="32">
+      <c r="D44" s="31">
         <v>5</v>
       </c>
-      <c r="E44" s="32">
+      <c r="E44" s="31">
         <v>1</v>
       </c>
       <c r="F44" s="18">
@@ -5140,16 +6097,16 @@
       </c>
     </row>
     <row r="45" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="32">
+      <c r="B45" s="31">
         <v>14</v>
       </c>
-      <c r="C45" s="46" t="s">
+      <c r="C45" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D45" s="32">
+      <c r="D45" s="31">
         <v>5</v>
       </c>
-      <c r="E45" s="32">
+      <c r="E45" s="31">
         <v>2</v>
       </c>
       <c r="F45" s="18">
@@ -5183,16 +6140,16 @@
       </c>
     </row>
     <row r="46" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="32">
+      <c r="B46" s="31">
         <v>15</v>
       </c>
-      <c r="C46" s="46" t="s">
+      <c r="C46" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D46" s="32">
+      <c r="D46" s="31">
         <v>5</v>
       </c>
-      <c r="E46" s="32">
+      <c r="E46" s="31">
         <v>3</v>
       </c>
       <c r="F46" s="18">
@@ -5226,16 +6183,16 @@
       </c>
     </row>
     <row r="47" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="32">
+      <c r="B47" s="31">
         <v>16</v>
       </c>
-      <c r="C47" s="46" t="s">
+      <c r="C47" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="32">
+      <c r="D47" s="31">
         <v>6</v>
       </c>
-      <c r="E47" s="32">
+      <c r="E47" s="31">
         <v>1</v>
       </c>
       <c r="F47" s="18">
@@ -5268,16 +6225,16 @@
       </c>
     </row>
     <row r="48" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="32">
+      <c r="B48" s="31">
         <v>17</v>
       </c>
-      <c r="C48" s="46" t="s">
+      <c r="C48" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D48" s="32">
+      <c r="D48" s="31">
         <v>6</v>
       </c>
-      <c r="E48" s="32">
+      <c r="E48" s="31">
         <v>2</v>
       </c>
       <c r="F48" s="18">
@@ -5310,16 +6267,16 @@
       </c>
     </row>
     <row r="49" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="32">
+      <c r="B49" s="31">
         <v>18</v>
       </c>
-      <c r="C49" s="46" t="s">
+      <c r="C49" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D49" s="32">
+      <c r="D49" s="31">
         <v>6</v>
       </c>
-      <c r="E49" s="32">
+      <c r="E49" s="31">
         <v>3</v>
       </c>
       <c r="F49" s="18">
@@ -5352,16 +6309,16 @@
       </c>
     </row>
     <row r="50" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="32">
+      <c r="B50" s="31">
         <v>19</v>
       </c>
-      <c r="C50" s="46" t="s">
+      <c r="C50" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D50" s="32">
+      <c r="D50" s="31">
         <v>7</v>
       </c>
-      <c r="E50" s="32">
+      <c r="E50" s="31">
         <v>1</v>
       </c>
       <c r="F50" s="18">
@@ -5394,16 +6351,16 @@
       </c>
     </row>
     <row r="51" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="32">
+      <c r="B51" s="31">
         <v>20</v>
       </c>
-      <c r="C51" s="46" t="s">
+      <c r="C51" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D51" s="32">
+      <c r="D51" s="31">
         <v>7</v>
       </c>
-      <c r="E51" s="32">
+      <c r="E51" s="31">
         <v>2</v>
       </c>
       <c r="F51" s="18">
@@ -5436,16 +6393,16 @@
       </c>
     </row>
     <row r="52" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="32">
+      <c r="B52" s="31">
         <v>21</v>
       </c>
-      <c r="C52" s="46" t="s">
+      <c r="C52" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D52" s="32">
+      <c r="D52" s="31">
         <v>7</v>
       </c>
-      <c r="E52" s="32">
+      <c r="E52" s="31">
         <v>3</v>
       </c>
       <c r="F52" s="18">
@@ -5478,16 +6435,16 @@
       </c>
     </row>
     <row r="53" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="32">
+      <c r="B53" s="31">
         <v>22</v>
       </c>
-      <c r="C53" s="46" t="s">
+      <c r="C53" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D53" s="32">
+      <c r="D53" s="31">
         <v>8</v>
       </c>
-      <c r="E53" s="32">
+      <c r="E53" s="31">
         <v>1</v>
       </c>
       <c r="F53" s="18">
@@ -5520,16 +6477,16 @@
       </c>
     </row>
     <row r="54" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="32">
+      <c r="B54" s="31">
         <v>23</v>
       </c>
-      <c r="C54" s="46" t="s">
+      <c r="C54" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D54" s="32">
+      <c r="D54" s="31">
         <v>8</v>
       </c>
-      <c r="E54" s="32">
+      <c r="E54" s="31">
         <v>2</v>
       </c>
       <c r="F54" s="18">
@@ -5562,16 +6519,16 @@
       </c>
     </row>
     <row r="55" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="32">
+      <c r="B55" s="31">
         <v>24</v>
       </c>
-      <c r="C55" s="46" t="s">
+      <c r="C55" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D55" s="32">
+      <c r="D55" s="31">
         <v>8</v>
       </c>
-      <c r="E55" s="32">
+      <c r="E55" s="31">
         <v>3</v>
       </c>
       <c r="F55" s="18">
@@ -5604,16 +6561,16 @@
       </c>
     </row>
     <row r="56" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="32">
+      <c r="B56" s="31">
         <v>25</v>
       </c>
-      <c r="C56" s="46" t="s">
+      <c r="C56" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D56" s="32">
+      <c r="D56" s="31">
         <v>9</v>
       </c>
-      <c r="E56" s="32">
+      <c r="E56" s="31">
         <v>1</v>
       </c>
       <c r="F56" s="18">
@@ -5646,16 +6603,16 @@
       </c>
     </row>
     <row r="57" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="32">
+      <c r="B57" s="31">
         <v>26</v>
       </c>
-      <c r="C57" s="46" t="s">
+      <c r="C57" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D57" s="32">
+      <c r="D57" s="31">
         <v>9</v>
       </c>
-      <c r="E57" s="32">
+      <c r="E57" s="31">
         <v>2</v>
       </c>
       <c r="F57" s="18">
@@ -5688,16 +6645,16 @@
       </c>
     </row>
     <row r="58" spans="2:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="32">
+      <c r="B58" s="31">
         <v>27</v>
       </c>
-      <c r="C58" s="46" t="s">
+      <c r="C58" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D58" s="32">
+      <c r="D58" s="31">
         <v>9</v>
       </c>
-      <c r="E58" s="32">
+      <c r="E58" s="31">
         <v>3</v>
       </c>
       <c r="F58" s="18">

</xml_diff>